<commit_message>
Added logic for age parameter in sorting
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -232,12 +232,18 @@
       <name val="Calibri"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+        <bgColor auto="1"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -250,16 +256,16 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </left>
       <right style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </right>
       <top style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </top>
       <bottom style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </bottom>
       <diagonal/>
     </border>
@@ -276,13 +282,13 @@
     <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="0" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
   </cellXfs>
@@ -302,6 +308,7 @@
       <rgbColor rgb="ffff00ff"/>
       <rgbColor rgb="ff00ffff"/>
       <rgbColor rgb="ff000000"/>
+      <rgbColor rgb="ffffffff"/>
       <rgbColor rgb="ffaaaaaa"/>
     </indexedColors>
   </colors>
@@ -453,9 +460,9 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="20000" dir="5400000">
+            <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="23000" dir="5400000">
               <a:srgbClr val="000000">
-                <a:alpha val="38000"/>
+                <a:alpha val="35000"/>
               </a:srgbClr>
             </a:outerShdw>
           </a:effectLst>
@@ -535,7 +542,7 @@
         </a:effectLst>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45719" tIns="45719" rIns="45719" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45718" tIns="45718" rIns="45718" bIns="45718" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr" upright="0">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -563,10 +570,10 @@
             </a:solidFill>
             <a:effectLst/>
             <a:uFillTx/>
-            <a:latin typeface="Calibri"/>
-            <a:ea typeface="Calibri"/>
-            <a:cs typeface="Calibri"/>
-            <a:sym typeface="Calibri"/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+            <a:sym typeface="Helvetica Neue"/>
           </a:defRPr>
         </a:defPPr>
         <a:lvl1pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
@@ -822,9 +829,9 @@
           <a:round/>
         </a:ln>
         <a:effectLst>
-          <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="20000" dir="5400000">
+          <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="23000" dir="5400000">
             <a:srgbClr val="000000">
-              <a:alpha val="38000"/>
+              <a:alpha val="35000"/>
             </a:srgbClr>
           </a:outerShdw>
         </a:effectLst>
@@ -1112,7 +1119,7 @@
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45719" tIns="45719" rIns="45719" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45718" tIns="45718" rIns="45718" bIns="45718" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -1140,10 +1147,10 @@
             </a:solidFill>
             <a:effectLst/>
             <a:uFillTx/>
-            <a:latin typeface="Calibri"/>
-            <a:ea typeface="Calibri"/>
-            <a:cs typeface="Calibri"/>
-            <a:sym typeface="Calibri"/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+            <a:sym typeface="Helvetica Neue"/>
           </a:defRPr>
         </a:defPPr>
         <a:lvl1pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
@@ -1404,7 +1411,7 @@
     <col min="5" max="5" width="16.3516" style="1" customWidth="1"/>
     <col min="6" max="8" width="10.8516" style="1" customWidth="1"/>
     <col min="9" max="15" width="4.85156" style="1" customWidth="1"/>
-    <col min="16" max="16" width="31.5781" style="1" customWidth="1"/>
+    <col min="16" max="16" width="31.6719" style="1" customWidth="1"/>
     <col min="17" max="256" width="10.8516" style="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1466,7 +1473,9 @@
       </c>
       <c r="M2" s="3"/>
       <c r="N2" s="3"/>
-      <c r="O2" s="3"/>
+      <c r="O2" s="4">
+        <v>5</v>
+      </c>
       <c r="P2" s="3"/>
     </row>
     <row r="3" ht="17" customHeight="1">
@@ -1497,7 +1506,9 @@
       </c>
       <c r="M3" s="3"/>
       <c r="N3" s="3"/>
-      <c r="O3" s="3"/>
+      <c r="O3" s="4">
+        <v>6</v>
+      </c>
       <c r="P3" s="3"/>
     </row>
     <row r="4" ht="17" customHeight="1">
@@ -1522,7 +1533,9 @@
       </c>
       <c r="M4" s="3"/>
       <c r="N4" s="3"/>
-      <c r="O4" s="3"/>
+      <c r="O4" s="4">
+        <v>7</v>
+      </c>
       <c r="P4" s="3"/>
     </row>
     <row r="5" ht="17" customHeight="1">
@@ -1553,7 +1566,9 @@
       </c>
       <c r="M5" s="3"/>
       <c r="N5" s="3"/>
-      <c r="O5" s="3"/>
+      <c r="O5" s="4">
+        <v>6</v>
+      </c>
       <c r="P5" s="3"/>
     </row>
     <row r="6" ht="17" customHeight="1">
@@ -1584,7 +1599,9 @@
       </c>
       <c r="M6" s="3"/>
       <c r="N6" s="3"/>
-      <c r="O6" s="3"/>
+      <c r="O6" s="4">
+        <v>6</v>
+      </c>
       <c r="P6" s="3"/>
     </row>
     <row r="7" ht="17" customHeight="1">
@@ -1615,7 +1632,9 @@
       </c>
       <c r="M7" s="3"/>
       <c r="N7" s="3"/>
-      <c r="O7" s="3"/>
+      <c r="O7" s="4">
+        <v>7</v>
+      </c>
       <c r="P7" s="3"/>
     </row>
     <row r="8" ht="17" customHeight="1">
@@ -1646,7 +1665,9 @@
       </c>
       <c r="M8" s="3"/>
       <c r="N8" s="3"/>
-      <c r="O8" s="3"/>
+      <c r="O8" s="4">
+        <v>5</v>
+      </c>
       <c r="P8" s="3"/>
     </row>
     <row r="9" ht="17" customHeight="1">
@@ -1677,7 +1698,9 @@
       </c>
       <c r="M9" s="3"/>
       <c r="N9" s="3"/>
-      <c r="O9" s="3"/>
+      <c r="O9" s="4">
+        <v>5</v>
+      </c>
       <c r="P9" s="3"/>
     </row>
     <row r="10" ht="17" customHeight="1">
@@ -1702,7 +1725,9 @@
       </c>
       <c r="M10" s="3"/>
       <c r="N10" s="3"/>
-      <c r="O10" s="3"/>
+      <c r="O10" s="4">
+        <v>7</v>
+      </c>
       <c r="P10" s="3"/>
     </row>
     <row r="11" ht="17" customHeight="1">
@@ -1733,7 +1758,9 @@
       </c>
       <c r="M11" s="3"/>
       <c r="N11" s="3"/>
-      <c r="O11" s="3"/>
+      <c r="O11" s="4">
+        <v>7</v>
+      </c>
       <c r="P11" s="3"/>
     </row>
     <row r="12" ht="17" customHeight="1">
@@ -1758,7 +1785,9 @@
       </c>
       <c r="M12" s="3"/>
       <c r="N12" s="3"/>
-      <c r="O12" s="3"/>
+      <c r="O12" s="4">
+        <v>7</v>
+      </c>
       <c r="P12" s="3"/>
     </row>
     <row r="13" ht="17" customHeight="1">
@@ -1783,7 +1812,9 @@
       </c>
       <c r="M13" s="3"/>
       <c r="N13" s="3"/>
-      <c r="O13" s="3"/>
+      <c r="O13" s="4">
+        <v>7</v>
+      </c>
       <c r="P13" s="3"/>
     </row>
     <row r="14" ht="17" customHeight="1">
@@ -1814,7 +1845,9 @@
       </c>
       <c r="M14" s="3"/>
       <c r="N14" s="3"/>
-      <c r="O14" s="3"/>
+      <c r="O14" s="4">
+        <v>6</v>
+      </c>
       <c r="P14" s="3"/>
     </row>
     <row r="15" ht="17" customHeight="1">
@@ -1839,7 +1872,9 @@
       </c>
       <c r="M15" s="3"/>
       <c r="N15" s="3"/>
-      <c r="O15" s="3"/>
+      <c r="O15" s="4">
+        <v>6</v>
+      </c>
       <c r="P15" s="3"/>
     </row>
     <row r="16" ht="17" customHeight="1">
@@ -1870,7 +1905,9 @@
       </c>
       <c r="M16" s="3"/>
       <c r="N16" s="3"/>
-      <c r="O16" s="3"/>
+      <c r="O16" s="4">
+        <v>7</v>
+      </c>
       <c r="P16" s="3"/>
     </row>
     <row r="17" ht="17" customHeight="1">
@@ -1901,7 +1938,9 @@
       </c>
       <c r="M17" s="3"/>
       <c r="N17" s="3"/>
-      <c r="O17" s="3"/>
+      <c r="O17" s="4">
+        <v>7</v>
+      </c>
       <c r="P17" s="3"/>
     </row>
     <row r="18" ht="17" customHeight="1">
@@ -1932,7 +1971,9 @@
       </c>
       <c r="M18" s="3"/>
       <c r="N18" s="3"/>
-      <c r="O18" s="3"/>
+      <c r="O18" s="4">
+        <v>6</v>
+      </c>
       <c r="P18" s="3"/>
     </row>
     <row r="19" ht="17" customHeight="1">
@@ -1963,7 +2004,9 @@
       </c>
       <c r="M19" s="3"/>
       <c r="N19" s="3"/>
-      <c r="O19" s="3"/>
+      <c r="O19" s="4">
+        <v>5</v>
+      </c>
       <c r="P19" s="3"/>
     </row>
     <row r="20" ht="17" customHeight="1">
@@ -1988,7 +2031,9 @@
       </c>
       <c r="M20" s="3"/>
       <c r="N20" s="3"/>
-      <c r="O20" s="3"/>
+      <c r="O20" s="4">
+        <v>6</v>
+      </c>
       <c r="P20" s="3"/>
     </row>
     <row r="21" ht="17" customHeight="1">
@@ -2019,7 +2064,9 @@
       </c>
       <c r="M21" s="3"/>
       <c r="N21" s="3"/>
-      <c r="O21" s="3"/>
+      <c r="O21" s="4">
+        <v>6</v>
+      </c>
       <c r="P21" s="3"/>
     </row>
     <row r="22" ht="17" customHeight="1">
@@ -2044,7 +2091,9 @@
       </c>
       <c r="M22" s="3"/>
       <c r="N22" s="3"/>
-      <c r="O22" s="3"/>
+      <c r="O22" s="4">
+        <v>5</v>
+      </c>
       <c r="P22" s="3"/>
     </row>
     <row r="23" ht="17" customHeight="1">
@@ -2075,7 +2124,9 @@
       </c>
       <c r="M23" s="3"/>
       <c r="N23" s="3"/>
-      <c r="O23" s="3"/>
+      <c r="O23" s="4">
+        <v>5</v>
+      </c>
       <c r="P23" s="3"/>
     </row>
     <row r="24" ht="17" customHeight="1">
@@ -2106,7 +2157,9 @@
       </c>
       <c r="M24" s="3"/>
       <c r="N24" s="3"/>
-      <c r="O24" s="3"/>
+      <c r="O24" s="4">
+        <v>6</v>
+      </c>
       <c r="P24" s="3"/>
     </row>
     <row r="25" ht="17" customHeight="1">
@@ -2137,7 +2190,9 @@
       </c>
       <c r="M25" s="3"/>
       <c r="N25" s="3"/>
-      <c r="O25" s="3"/>
+      <c r="O25" s="4">
+        <v>7</v>
+      </c>
       <c r="P25" s="3"/>
     </row>
     <row r="26" ht="17" customHeight="1">
@@ -2162,7 +2217,9 @@
       </c>
       <c r="M26" s="3"/>
       <c r="N26" s="3"/>
-      <c r="O26" s="3"/>
+      <c r="O26" s="4">
+        <v>7</v>
+      </c>
       <c r="P26" s="3"/>
     </row>
     <row r="27" ht="17" customHeight="1">
@@ -2193,7 +2250,9 @@
       </c>
       <c r="M27" s="3"/>
       <c r="N27" s="3"/>
-      <c r="O27" s="3"/>
+      <c r="O27" s="4">
+        <v>6</v>
+      </c>
       <c r="P27" s="3"/>
     </row>
     <row r="28" ht="17" customHeight="1">
@@ -2224,7 +2283,9 @@
       </c>
       <c r="M28" s="3"/>
       <c r="N28" s="3"/>
-      <c r="O28" s="3"/>
+      <c r="O28" s="4">
+        <v>5</v>
+      </c>
       <c r="P28" s="3"/>
     </row>
     <row r="29" ht="17" customHeight="1">
@@ -2249,7 +2310,9 @@
       </c>
       <c r="M29" s="3"/>
       <c r="N29" s="3"/>
-      <c r="O29" s="3"/>
+      <c r="O29" s="4">
+        <v>6</v>
+      </c>
       <c r="P29" s="3"/>
     </row>
     <row r="30" ht="17" customHeight="1">
@@ -2280,7 +2343,9 @@
       </c>
       <c r="M30" s="3"/>
       <c r="N30" s="3"/>
-      <c r="O30" s="3"/>
+      <c r="O30" s="4">
+        <v>6</v>
+      </c>
       <c r="P30" s="3"/>
     </row>
     <row r="31" ht="17" customHeight="1">
@@ -2305,7 +2370,9 @@
       </c>
       <c r="M31" s="3"/>
       <c r="N31" s="3"/>
-      <c r="O31" s="3"/>
+      <c r="O31" s="4">
+        <v>7</v>
+      </c>
       <c r="P31" s="3"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
player request logic added
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="66">
   <si>
     <t>Team#</t>
   </si>
@@ -38,6 +38,9 @@
   </si>
   <si>
     <t>Binder</t>
+  </si>
+  <si>
+    <t>Req Player Ethan Garcia</t>
   </si>
   <si>
     <t>Christopher</t>
@@ -1476,17 +1479,19 @@
       <c r="O2" s="4">
         <v>5</v>
       </c>
-      <c r="P2" s="3"/>
+      <c r="P2" t="s" s="2">
+        <v>9</v>
+      </c>
     </row>
     <row r="3" ht="17" customHeight="1">
       <c r="A3" s="3"/>
       <c r="B3" s="3"/>
       <c r="C3" s="3"/>
       <c r="D3" t="s" s="2">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E3" t="s" s="2">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F3" s="4">
         <v>3</v>
@@ -1516,10 +1521,10 @@
       <c r="B4" s="3"/>
       <c r="C4" s="3"/>
       <c r="D4" t="s" s="2">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E4" t="s" s="2">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F4" s="3"/>
       <c r="G4" s="3"/>
@@ -1543,10 +1548,10 @@
       <c r="B5" s="3"/>
       <c r="C5" s="3"/>
       <c r="D5" t="s" s="2">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E5" t="s" s="2">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="F5" s="4">
         <v>3</v>
@@ -1576,10 +1581,10 @@
       <c r="B6" s="3"/>
       <c r="C6" s="3"/>
       <c r="D6" t="s" s="2">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E6" t="s" s="2">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="F6" s="4">
         <v>2</v>
@@ -1609,10 +1614,10 @@
       <c r="B7" s="3"/>
       <c r="C7" s="3"/>
       <c r="D7" t="s" s="2">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E7" t="s" s="2">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F7" s="4">
         <v>2.5</v>
@@ -1642,10 +1647,10 @@
       <c r="B8" s="3"/>
       <c r="C8" s="3"/>
       <c r="D8" t="s" s="2">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E8" t="s" s="2">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F8" s="4">
         <v>2</v>
@@ -1675,10 +1680,10 @@
       <c r="B9" s="3"/>
       <c r="C9" s="3"/>
       <c r="D9" t="s" s="2">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E9" t="s" s="2">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="F9" s="4">
         <v>2.5</v>
@@ -1708,10 +1713,10 @@
       <c r="B10" s="3"/>
       <c r="C10" s="3"/>
       <c r="D10" t="s" s="2">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E10" t="s" s="2">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="F10" s="3"/>
       <c r="G10" s="3"/>
@@ -1735,10 +1740,10 @@
       <c r="B11" s="3"/>
       <c r="C11" s="3"/>
       <c r="D11" t="s" s="2">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="E11" t="s" s="2">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="F11" s="4">
         <v>2</v>
@@ -1768,10 +1773,10 @@
       <c r="B12" s="3"/>
       <c r="C12" s="3"/>
       <c r="D12" t="s" s="2">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="E12" t="s" s="2">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="F12" s="3"/>
       <c r="G12" s="3"/>
@@ -1795,10 +1800,10 @@
       <c r="B13" s="3"/>
       <c r="C13" s="3"/>
       <c r="D13" t="s" s="2">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="E13" t="s" s="2">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="F13" s="3"/>
       <c r="G13" s="3"/>
@@ -1822,10 +1827,10 @@
       <c r="B14" s="3"/>
       <c r="C14" s="3"/>
       <c r="D14" t="s" s="2">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="E14" t="s" s="2">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="F14" s="4">
         <v>2</v>
@@ -1855,10 +1860,10 @@
       <c r="B15" s="3"/>
       <c r="C15" s="3"/>
       <c r="D15" t="s" s="2">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="E15" t="s" s="2">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="F15" s="3"/>
       <c r="G15" s="3"/>
@@ -1882,10 +1887,10 @@
       <c r="B16" s="3"/>
       <c r="C16" s="3"/>
       <c r="D16" t="s" s="2">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="E16" t="s" s="2">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="F16" s="4">
         <v>3</v>
@@ -1915,10 +1920,10 @@
       <c r="B17" s="3"/>
       <c r="C17" s="3"/>
       <c r="D17" t="s" s="2">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="E17" t="s" s="2">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="F17" s="4">
         <v>2.5</v>
@@ -1948,10 +1953,10 @@
       <c r="B18" s="3"/>
       <c r="C18" s="3"/>
       <c r="D18" t="s" s="2">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="E18" t="s" s="2">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="F18" s="4">
         <v>2.5</v>
@@ -1981,10 +1986,10 @@
       <c r="B19" s="3"/>
       <c r="C19" s="3"/>
       <c r="D19" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="E19" t="s" s="2">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="F19" s="4">
         <v>2</v>
@@ -2014,10 +2019,10 @@
       <c r="B20" s="3"/>
       <c r="C20" s="3"/>
       <c r="D20" t="s" s="2">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="E20" t="s" s="2">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="F20" s="3"/>
       <c r="G20" s="3"/>
@@ -2041,10 +2046,10 @@
       <c r="B21" s="3"/>
       <c r="C21" s="3"/>
       <c r="D21" t="s" s="2">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="E21" t="s" s="2">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="F21" s="4">
         <v>3</v>
@@ -2074,10 +2079,10 @@
       <c r="B22" s="3"/>
       <c r="C22" s="3"/>
       <c r="D22" t="s" s="2">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="E22" t="s" s="2">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="F22" s="3"/>
       <c r="G22" s="3"/>
@@ -2101,10 +2106,10 @@
       <c r="B23" s="3"/>
       <c r="C23" s="3"/>
       <c r="D23" t="s" s="2">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="E23" t="s" s="2">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="F23" s="4">
         <v>1.5</v>
@@ -2134,10 +2139,10 @@
       <c r="B24" s="3"/>
       <c r="C24" s="3"/>
       <c r="D24" t="s" s="2">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="E24" t="s" s="2">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="F24" s="4">
         <v>3</v>
@@ -2167,10 +2172,10 @@
       <c r="B25" s="3"/>
       <c r="C25" s="3"/>
       <c r="D25" t="s" s="2">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="E25" t="s" s="2">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="F25" s="4">
         <v>2.5</v>
@@ -2200,10 +2205,10 @@
       <c r="B26" s="3"/>
       <c r="C26" s="3"/>
       <c r="D26" t="s" s="2">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="E26" t="s" s="2">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="F26" s="3"/>
       <c r="G26" s="3"/>
@@ -2227,10 +2232,10 @@
       <c r="B27" s="3"/>
       <c r="C27" s="3"/>
       <c r="D27" t="s" s="2">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="E27" t="s" s="2">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="F27" s="4">
         <v>2.5</v>
@@ -2260,10 +2265,10 @@
       <c r="B28" s="3"/>
       <c r="C28" s="3"/>
       <c r="D28" t="s" s="2">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="E28" t="s" s="2">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="F28" s="4">
         <v>2</v>
@@ -2293,10 +2298,10 @@
       <c r="B29" s="3"/>
       <c r="C29" s="3"/>
       <c r="D29" t="s" s="2">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="E29" t="s" s="2">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="F29" s="3"/>
       <c r="G29" s="3"/>
@@ -2320,10 +2325,10 @@
       <c r="B30" s="3"/>
       <c r="C30" s="3"/>
       <c r="D30" t="s" s="2">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="E30" t="s" s="2">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="F30" s="4">
         <v>2.5</v>
@@ -2353,10 +2358,10 @@
       <c r="B31" s="3"/>
       <c r="C31" s="3"/>
       <c r="D31" t="s" s="2">
+        <v>65</v>
+      </c>
+      <c r="E31" t="s" s="2">
         <v>64</v>
-      </c>
-      <c r="E31" t="s" s="2">
-        <v>63</v>
       </c>
       <c r="F31" s="3"/>
       <c r="G31" s="3"/>

</xml_diff>

<commit_message>
added coach request logic
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="67">
   <si>
     <t>Team#</t>
   </si>
@@ -83,6 +83,9 @@
   </si>
   <si>
     <t>McClung</t>
+  </si>
+  <si>
+    <t>Req coach 3</t>
   </si>
   <si>
     <t>Daniel</t>
@@ -1706,17 +1709,19 @@
       <c r="O9" s="4">
         <v>5</v>
       </c>
-      <c r="P9" s="3"/>
+      <c r="P9" t="s" s="2">
+        <v>24</v>
+      </c>
     </row>
     <row r="10" ht="17" customHeight="1">
       <c r="A10" s="3"/>
       <c r="B10" s="3"/>
       <c r="C10" s="3"/>
       <c r="D10" t="s" s="2">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="E10" t="s" s="2">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="F10" s="3"/>
       <c r="G10" s="3"/>
@@ -1740,10 +1745,10 @@
       <c r="B11" s="3"/>
       <c r="C11" s="3"/>
       <c r="D11" t="s" s="2">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E11" t="s" s="2">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="F11" s="4">
         <v>2</v>
@@ -1773,10 +1778,10 @@
       <c r="B12" s="3"/>
       <c r="C12" s="3"/>
       <c r="D12" t="s" s="2">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="E12" t="s" s="2">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="F12" s="3"/>
       <c r="G12" s="3"/>
@@ -1800,10 +1805,10 @@
       <c r="B13" s="3"/>
       <c r="C13" s="3"/>
       <c r="D13" t="s" s="2">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="E13" t="s" s="2">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="F13" s="3"/>
       <c r="G13" s="3"/>
@@ -1827,10 +1832,10 @@
       <c r="B14" s="3"/>
       <c r="C14" s="3"/>
       <c r="D14" t="s" s="2">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="E14" t="s" s="2">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="F14" s="4">
         <v>2</v>
@@ -1860,10 +1865,10 @@
       <c r="B15" s="3"/>
       <c r="C15" s="3"/>
       <c r="D15" t="s" s="2">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="E15" t="s" s="2">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="F15" s="3"/>
       <c r="G15" s="3"/>
@@ -1887,10 +1892,10 @@
       <c r="B16" s="3"/>
       <c r="C16" s="3"/>
       <c r="D16" t="s" s="2">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E16" t="s" s="2">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="F16" s="4">
         <v>3</v>
@@ -1920,10 +1925,10 @@
       <c r="B17" s="3"/>
       <c r="C17" s="3"/>
       <c r="D17" t="s" s="2">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="E17" t="s" s="2">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="F17" s="4">
         <v>2.5</v>
@@ -1953,10 +1958,10 @@
       <c r="B18" s="3"/>
       <c r="C18" s="3"/>
       <c r="D18" t="s" s="2">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="E18" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="F18" s="4">
         <v>2.5</v>
@@ -1986,10 +1991,10 @@
       <c r="B19" s="3"/>
       <c r="C19" s="3"/>
       <c r="D19" t="s" s="2">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="E19" t="s" s="2">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="F19" s="4">
         <v>2</v>
@@ -2019,10 +2024,10 @@
       <c r="B20" s="3"/>
       <c r="C20" s="3"/>
       <c r="D20" t="s" s="2">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="E20" t="s" s="2">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="F20" s="3"/>
       <c r="G20" s="3"/>
@@ -2046,10 +2051,10 @@
       <c r="B21" s="3"/>
       <c r="C21" s="3"/>
       <c r="D21" t="s" s="2">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="E21" t="s" s="2">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="F21" s="4">
         <v>3</v>
@@ -2079,10 +2084,10 @@
       <c r="B22" s="3"/>
       <c r="C22" s="3"/>
       <c r="D22" t="s" s="2">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="E22" t="s" s="2">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="F22" s="3"/>
       <c r="G22" s="3"/>
@@ -2106,10 +2111,10 @@
       <c r="B23" s="3"/>
       <c r="C23" s="3"/>
       <c r="D23" t="s" s="2">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="E23" t="s" s="2">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="F23" s="4">
         <v>1.5</v>
@@ -2139,10 +2144,10 @@
       <c r="B24" s="3"/>
       <c r="C24" s="3"/>
       <c r="D24" t="s" s="2">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="E24" t="s" s="2">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="F24" s="4">
         <v>3</v>
@@ -2172,10 +2177,10 @@
       <c r="B25" s="3"/>
       <c r="C25" s="3"/>
       <c r="D25" t="s" s="2">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="E25" t="s" s="2">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="F25" s="4">
         <v>2.5</v>
@@ -2205,10 +2210,10 @@
       <c r="B26" s="3"/>
       <c r="C26" s="3"/>
       <c r="D26" t="s" s="2">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="E26" t="s" s="2">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="F26" s="3"/>
       <c r="G26" s="3"/>
@@ -2232,10 +2237,10 @@
       <c r="B27" s="3"/>
       <c r="C27" s="3"/>
       <c r="D27" t="s" s="2">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="E27" t="s" s="2">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="F27" s="4">
         <v>2.5</v>
@@ -2265,10 +2270,10 @@
       <c r="B28" s="3"/>
       <c r="C28" s="3"/>
       <c r="D28" t="s" s="2">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="E28" t="s" s="2">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="F28" s="4">
         <v>2</v>
@@ -2298,10 +2303,10 @@
       <c r="B29" s="3"/>
       <c r="C29" s="3"/>
       <c r="D29" t="s" s="2">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="E29" t="s" s="2">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="F29" s="3"/>
       <c r="G29" s="3"/>
@@ -2325,10 +2330,10 @@
       <c r="B30" s="3"/>
       <c r="C30" s="3"/>
       <c r="D30" t="s" s="2">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="E30" t="s" s="2">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="F30" s="4">
         <v>2.5</v>
@@ -2358,10 +2363,10 @@
       <c r="B31" s="3"/>
       <c r="C31" s="3"/>
       <c r="D31" t="s" s="2">
+        <v>66</v>
+      </c>
+      <c r="E31" t="s" s="2">
         <v>65</v>
-      </c>
-      <c r="E31" t="s" s="2">
-        <v>64</v>
       </c>
       <c r="F31" s="3"/>
       <c r="G31" s="3"/>

</xml_diff>